<commit_message>
Brazil dataset - changed columns names
</commit_message>
<xml_diff>
--- a/data/Brazilian_Weather_Stations-Temperature_1961-1990.xlsx
+++ b/data/Brazilian_Weather_Stations-Temperature_1961-1990.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Studies\MSc\Research\Graph_Signal_Processing\src\GSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F51BE1E-0391-4225-B971-DD8A56224040}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E048C93-7876-4C39-B65B-9FF324A99961}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="406" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2685,7 +2685,7 @@
     <t>Dec</t>
   </si>
   <si>
-    <t>Annual</t>
+    <t>Ann</t>
   </si>
 </sst>
 </file>
@@ -3463,7 +3463,8 @@
   <dimension ref="A1:S300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>